<commit_message>
f/mmcdaniel-bloodGas: Finalize model and fine tune gas solubilities
</commit_message>
<xml_diff>
--- a/share/data/BioGears.xlsx
+++ b/share/data/BioGears.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProjectPrograms\BioGears\core-lite\build2019\runtime\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProjectPrograms\BioGears\core-lite\build\runtime\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2232,10 +2232,10 @@
     <t>40.0 mL/min kg</t>
   </si>
   <si>
-    <t>0.6475 1/atm</t>
-  </si>
-  <si>
-    <t>0.02485 1/atm</t>
+    <t>0.0233 1/atm</t>
+  </si>
+  <si>
+    <t>0.557 1/atm</t>
   </si>
 </sst>
 </file>
@@ -4931,7 +4931,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="N16" sqref="N16"/>
+      <selection pane="bottomRight" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -8221,7 +8221,7 @@
         <v>73</v>
       </c>
       <c r="B12" s="104" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="C12" s="104"/>
       <c r="D12" s="104"/>
@@ -8245,7 +8245,7 @@
       <c r="L12" s="104"/>
       <c r="M12" s="104"/>
       <c r="N12" s="101" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="O12" s="104"/>
       <c r="P12" s="104"/>

</xml_diff>

<commit_message>
f/mmcdaniel-liteActions: Fix acetominophen substance definition
</commit_message>
<xml_diff>
--- a/share/data/BioGears.xlsx
+++ b/share/data/BioGears.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProjectPrograms\BioGears\core-lite\build\runtime\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProjectPrograms\BioGears\core-lite\share\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2382,9 +2382,6 @@
     <t>0.3 1/hr</t>
   </si>
   <si>
-    <t>[0.05; 2.75 ug/mL]</t>
-  </si>
-  <si>
     <t>[0.05; 1.5 ug/mL]</t>
   </si>
   <si>
@@ -2428,6 +2425,9 @@
   </si>
   <si>
     <t>30 mg/min</t>
+  </si>
+  <si>
+    <t>[0.55; 2.75 ug/mL]</t>
   </si>
 </sst>
 </file>
@@ -5277,7 +5277,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="BZ15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="R29" sqref="R29"/>
+      <selection pane="bottomRight" activeCell="BZ49" sqref="BZ49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -14123,7 +14123,7 @@
     </row>
     <row r="29" spans="1:200" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="80" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="B29" s="98"/>
       <c r="C29" s="98"/>
@@ -14142,37 +14142,37 @@
       <c r="P29" s="98"/>
       <c r="Q29" s="98"/>
       <c r="R29" s="87" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="S29" s="87"/>
       <c r="T29" s="87"/>
       <c r="U29" s="87"/>
       <c r="V29" s="87" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="W29" s="81" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="X29" s="87" t="s">
         <v>262</v>
       </c>
       <c r="Y29" s="87" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="Z29" s="83" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="AA29" s="87"/>
       <c r="AB29" s="87"/>
       <c r="AC29" s="87"/>
       <c r="AD29" s="83" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="AE29" s="87"/>
       <c r="AF29" s="87"/>
       <c r="AG29" s="87"/>
       <c r="AH29" s="83" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="AI29" s="89"/>
       <c r="AJ29" s="89"/>
@@ -14190,13 +14190,13 @@
       <c r="AV29" s="161"/>
       <c r="AW29" s="161"/>
       <c r="AX29" s="166" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="AY29" s="166"/>
       <c r="AZ29" s="166"/>
       <c r="BA29" s="166"/>
       <c r="BB29" s="166" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="BC29" s="166">
         <v>0</v>
@@ -14205,13 +14205,13 @@
         <v>262</v>
       </c>
       <c r="BE29" s="166" t="s">
+        <v>790</v>
+      </c>
+      <c r="BF29" s="166" t="s">
         <v>791</v>
       </c>
-      <c r="BF29" s="166" t="s">
+      <c r="BG29" s="166" t="s">
         <v>792</v>
-      </c>
-      <c r="BG29" s="166" t="s">
-        <v>793</v>
       </c>
       <c r="BH29" s="166" t="s">
         <v>262</v>
@@ -14220,18 +14220,18 @@
         <v>331</v>
       </c>
       <c r="BJ29" s="166" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="BK29" s="166" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="BL29" s="166"/>
       <c r="BM29" s="166"/>
       <c r="BN29" s="166" t="s">
+        <v>794</v>
+      </c>
+      <c r="BO29" s="166" t="s">
         <v>795</v>
-      </c>
-      <c r="BO29" s="166" t="s">
-        <v>796</v>
       </c>
       <c r="BP29" s="166" t="s">
         <v>262</v>
@@ -14244,7 +14244,7 @@
       <c r="BT29" s="166"/>
       <c r="BU29" s="166"/>
       <c r="BV29" s="166" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="BW29" s="166"/>
       <c r="BX29" s="166"/>
@@ -14327,7 +14327,7 @@
       <c r="EW29" s="106"/>
       <c r="EX29" s="106"/>
       <c r="EY29" s="176" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="EZ29" s="176"/>
       <c r="FA29" s="176"/>
@@ -18731,7 +18731,7 @@
       <c r="BX45" s="166"/>
       <c r="BY45" s="229"/>
       <c r="BZ45" s="110" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="CA45" s="110" t="s">
         <v>699</v>
@@ -19767,7 +19767,7 @@
         <v>260</v>
       </c>
       <c r="BZ49" s="110" t="s">
-        <v>782</v>
+        <v>797</v>
       </c>
       <c r="CA49" s="110" t="s">
         <v>699</v>
@@ -19806,7 +19806,7 @@
       <c r="CW49" s="110"/>
       <c r="CX49" s="110"/>
       <c r="CY49" s="110" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="CZ49" s="110"/>
       <c r="DA49" s="110"/>
@@ -20806,7 +20806,7 @@
       <c r="CG53" s="110"/>
       <c r="CH53" s="110"/>
       <c r="CI53" s="110" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="CJ53" s="110"/>
       <c r="CK53" s="110"/>
@@ -20830,7 +20830,7 @@
       <c r="CW53" s="110"/>
       <c r="CX53" s="110"/>
       <c r="CY53" s="110" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="CZ53" s="110"/>
       <c r="DA53" s="110"/>

</xml_diff>